<commit_message>
revise filter stations test
</commit_message>
<xml_diff>
--- a/Test Cases.xlsx
+++ b/Test Cases.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/25750dbe804f304d/Documents/LOCQ/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="21" documentId="8_{65A7F19E-5B5C-4DEC-8583-D59D302DE621}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7188EC74-4DB1-4B4F-99EA-E56AD9CBAA27}"/>
+  <xr:revisionPtr revIDLastSave="24" documentId="8_{65A7F19E-5B5C-4DEC-8583-D59D302DE621}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{05FB02F3-37F8-464E-A45D-216CC628DE0E}"/>
   <bookViews>
-    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="16305" xr2:uid="{500269A6-E25E-4BF0-A8C2-6D6766C0E225}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="2" xr2:uid="{500269A6-E25E-4BF0-A8C2-6D6766C0E225}"/>
   </bookViews>
   <sheets>
     <sheet name="6 LoginPage" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">'6 LoginPage'!$A$2:$F$59</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="1">'7 POS Payment'!$A$2:$F$14</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="1">'7 POS Payment'!$A$2:$F$17</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="2">'8 Log Ticket'!$A$1:$B$23</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
@@ -603,7 +603,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -677,23 +677,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" indent="2"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -712,6 +704,12 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="2"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="2"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -777,6 +775,10 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1078,8 +1080,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{464F6AF7-54A2-483B-8E47-4D01591E3850}">
   <dimension ref="A2:F59"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="60" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView view="pageBreakPreview" topLeftCell="A40" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="B55" sqref="B55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1096,77 +1098,77 @@
       <c r="A2" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="31" t="s">
+      <c r="B2" s="41" t="s">
         <v>70</v>
       </c>
-      <c r="C2" s="31"/>
-      <c r="D2" s="31"/>
-      <c r="E2" s="31"/>
-      <c r="F2" s="31"/>
+      <c r="C2" s="41"/>
+      <c r="D2" s="41"/>
+      <c r="E2" s="41"/>
+      <c r="F2" s="41"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="25" t="s">
         <v>68</v>
       </c>
-      <c r="B3" s="31" t="s">
+      <c r="B3" s="41" t="s">
         <v>69</v>
       </c>
-      <c r="C3" s="31"/>
-      <c r="D3" s="31"/>
-      <c r="E3" s="31"/>
-      <c r="F3" s="31"/>
+      <c r="C3" s="41"/>
+      <c r="D3" s="41"/>
+      <c r="E3" s="41"/>
+      <c r="F3" s="41"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="25" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="31" t="s">
+      <c r="B4" s="41" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="31"/>
-      <c r="D4" s="31"/>
-      <c r="E4" s="31"/>
-      <c r="F4" s="31"/>
+      <c r="C4" s="41"/>
+      <c r="D4" s="41"/>
+      <c r="E4" s="41"/>
+      <c r="F4" s="41"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="32">
+      <c r="B5" s="42">
         <v>45435</v>
       </c>
-      <c r="C5" s="31"/>
-      <c r="D5" s="31"/>
-      <c r="E5" s="31"/>
-      <c r="F5" s="31"/>
+      <c r="C5" s="41"/>
+      <c r="D5" s="41"/>
+      <c r="E5" s="41"/>
+      <c r="F5" s="41"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="31"/>
-      <c r="C6" s="31"/>
-      <c r="D6" s="31"/>
-      <c r="E6" s="31"/>
-      <c r="F6" s="31"/>
+      <c r="B6" s="41"/>
+      <c r="C6" s="41"/>
+      <c r="D6" s="41"/>
+      <c r="E6" s="41"/>
+      <c r="F6" s="41"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="25" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="31"/>
-      <c r="C7" s="31"/>
-      <c r="D7" s="31"/>
-      <c r="E7" s="31"/>
-      <c r="F7" s="31"/>
+      <c r="B7" s="41"/>
+      <c r="C7" s="41"/>
+      <c r="D7" s="41"/>
+      <c r="E7" s="41"/>
+      <c r="F7" s="41"/>
     </row>
     <row r="8" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="33"/>
-      <c r="B8" s="33"/>
-      <c r="C8" s="33"/>
-      <c r="D8" s="33"/>
-      <c r="E8" s="33"/>
-      <c r="F8" s="33"/>
+      <c r="A8" s="31"/>
+      <c r="B8" s="31"/>
+      <c r="C8" s="31"/>
+      <c r="D8" s="31"/>
+      <c r="E8" s="31"/>
+      <c r="F8" s="31"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="17" t="s">
@@ -1590,7 +1592,7 @@
       <c r="A33" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="B33" s="34"/>
+      <c r="B33" s="2"/>
       <c r="C33" s="11" t="s">
         <v>5</v>
       </c>
@@ -1723,7 +1725,7 @@
       <c r="D40" s="29" t="s">
         <v>18</v>
       </c>
-      <c r="E40" s="35" t="s">
+      <c r="E40" s="32" t="s">
         <v>19</v>
       </c>
       <c r="F40" s="30" t="s">
@@ -1829,7 +1831,7 @@
       <c r="D46" s="29" t="s">
         <v>18</v>
       </c>
-      <c r="E46" s="35" t="s">
+      <c r="E46" s="32" t="s">
         <v>19</v>
       </c>
       <c r="F46" s="30" t="s">
@@ -1935,7 +1937,7 @@
       <c r="D52" s="29" t="s">
         <v>18</v>
       </c>
-      <c r="E52" s="35" t="s">
+      <c r="E52" s="32" t="s">
         <v>19</v>
       </c>
       <c r="F52" s="30" t="s">
@@ -2078,7 +2080,7 @@
     <mergeCell ref="B6:F6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup scale="44" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2086,8 +2088,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6BF5D2C4-E555-434B-AC88-BFE623E45F2F}">
   <dimension ref="A2:F17"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2104,77 +2106,77 @@
       <c r="A2" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="31" t="s">
+      <c r="B2" s="41" t="s">
         <v>67</v>
       </c>
-      <c r="C2" s="31"/>
-      <c r="D2" s="31"/>
-      <c r="E2" s="31"/>
-      <c r="F2" s="31"/>
+      <c r="C2" s="41"/>
+      <c r="D2" s="41"/>
+      <c r="E2" s="41"/>
+      <c r="F2" s="41"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="25" t="s">
         <v>68</v>
       </c>
-      <c r="B3" s="31" t="s">
+      <c r="B3" s="41" t="s">
         <v>66</v>
       </c>
-      <c r="C3" s="31"/>
-      <c r="D3" s="31"/>
-      <c r="E3" s="31"/>
-      <c r="F3" s="31"/>
+      <c r="C3" s="41"/>
+      <c r="D3" s="41"/>
+      <c r="E3" s="41"/>
+      <c r="F3" s="41"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="25" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="31" t="s">
+      <c r="B4" s="41" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="31"/>
-      <c r="D4" s="31"/>
-      <c r="E4" s="31"/>
-      <c r="F4" s="31"/>
+      <c r="C4" s="41"/>
+      <c r="D4" s="41"/>
+      <c r="E4" s="41"/>
+      <c r="F4" s="41"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="32">
+      <c r="B5" s="42">
         <v>45435</v>
       </c>
-      <c r="C5" s="31"/>
-      <c r="D5" s="31"/>
-      <c r="E5" s="31"/>
-      <c r="F5" s="31"/>
+      <c r="C5" s="41"/>
+      <c r="D5" s="41"/>
+      <c r="E5" s="41"/>
+      <c r="F5" s="41"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="31"/>
-      <c r="C6" s="31"/>
-      <c r="D6" s="31"/>
-      <c r="E6" s="31"/>
-      <c r="F6" s="31"/>
+      <c r="B6" s="41"/>
+      <c r="C6" s="41"/>
+      <c r="D6" s="41"/>
+      <c r="E6" s="41"/>
+      <c r="F6" s="41"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="25" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="31"/>
-      <c r="C7" s="31"/>
-      <c r="D7" s="31"/>
-      <c r="E7" s="31"/>
-      <c r="F7" s="31"/>
+      <c r="B7" s="41"/>
+      <c r="C7" s="41"/>
+      <c r="D7" s="41"/>
+      <c r="E7" s="41"/>
+      <c r="F7" s="41"/>
     </row>
     <row r="8" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="33"/>
-      <c r="B8" s="33"/>
-      <c r="C8" s="33"/>
-      <c r="D8" s="33"/>
-      <c r="E8" s="33"/>
-      <c r="F8" s="33"/>
+      <c r="A8" s="31"/>
+      <c r="B8" s="31"/>
+      <c r="C8" s="31"/>
+      <c r="D8" s="31"/>
+      <c r="E8" s="31"/>
+      <c r="F8" s="31"/>
     </row>
     <row r="9" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A9" s="17" t="s">
@@ -2199,7 +2201,6 @@
       <c r="B10" s="10" t="s">
         <v>73</v>
       </c>
-      <c r="C10" s="37"/>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
       <c r="F10" s="4"/>
@@ -2323,36 +2324,36 @@
       </c>
     </row>
     <row r="17" spans="1:6" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="38">
+      <c r="A17" s="34">
         <v>6</v>
       </c>
-      <c r="B17" s="39" t="s">
+      <c r="B17" s="35" t="s">
         <v>90</v>
       </c>
-      <c r="C17" s="40" t="s">
+      <c r="C17" s="36" t="s">
         <v>15</v>
       </c>
-      <c r="D17" s="41" t="s">
+      <c r="D17" s="37" t="s">
         <v>91</v>
       </c>
-      <c r="E17" s="41" t="s">
+      <c r="E17" s="37" t="s">
         <v>92</v>
       </c>
-      <c r="F17" s="42" t="s">
+      <c r="F17" s="38" t="s">
         <v>16</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="B7:F7"/>
     <mergeCell ref="B2:F2"/>
     <mergeCell ref="B3:F3"/>
     <mergeCell ref="B4:F4"/>
     <mergeCell ref="B5:F5"/>
     <mergeCell ref="B6:F6"/>
-    <mergeCell ref="B7:F7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup scale="44" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2360,8 +2361,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A29396FC-423E-4230-98C7-54E58472021C}">
   <dimension ref="A2:I10"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" zoomScale="115" zoomScaleNormal="100" zoomScaleSheetLayoutView="115" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="115" zoomScaleNormal="100" zoomScaleSheetLayoutView="115" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2372,7 +2373,7 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="43" t="s">
+      <c r="A2" s="39" t="s">
         <v>93</v>
       </c>
       <c r="B2" t="s">
@@ -2383,10 +2384,10 @@
       </c>
     </row>
     <row r="3" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="43" t="s">
+      <c r="A3" s="39" t="s">
         <v>96</v>
       </c>
-      <c r="B3" s="36" t="s">
+      <c r="B3" s="33" t="s">
         <v>97</v>
       </c>
       <c r="I3" t="s">
@@ -2394,10 +2395,10 @@
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="43" t="s">
+      <c r="A4" s="39" t="s">
         <v>98</v>
       </c>
-      <c r="B4" s="44" t="s">
+      <c r="B4" s="40" t="s">
         <v>99</v>
       </c>
     </row>
@@ -2412,13 +2413,13 @@
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="43"/>
+      <c r="A7" s="39"/>
       <c r="B7" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="43" t="s">
+      <c r="A8" s="39" t="s">
         <v>103</v>
       </c>
       <c r="B8" t="s">
@@ -2426,7 +2427,7 @@
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="43" t="s">
+      <c r="A9" s="39" t="s">
         <v>105</v>
       </c>
       <c r="B9" t="s">
@@ -2434,7 +2435,7 @@
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="43" t="s">
+      <c r="A10" s="39" t="s">
         <v>107</v>
       </c>
     </row>

</xml_diff>